<commit_message>
updating github repo for class
</commit_message>
<xml_diff>
--- a/00-course-info/weekly-outline.xlsx
+++ b/00-course-info/weekly-outline.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/erobin17_calpoly_edu/Documents/stat365-calpoly/00-course-info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1020" documentId="11_F25DC773A252ABDACC1048BFF9586A525BDE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2E8433D-1507-4E1D-AF76-C45D47D6F7A5}"/>
+  <xr:revisionPtr revIDLastSave="1260" documentId="11_F25DC773A252ABDACC1048BFF9586A525BDE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3BE4917-66DB-46C4-8BDC-C3BC7F67A389}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Class-Schedule" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Resources" sheetId="1" r:id="rId1"/>
+    <sheet name="Resrouces" sheetId="2" r:id="rId2"/>
+    <sheet name="2023" sheetId="3" r:id="rId3"/>
+    <sheet name="2024" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="232">
   <si>
     <t>Date</t>
   </si>
@@ -591,13 +592,145 @@
   </si>
   <si>
     <t>Descriptive Statistics + Tables</t>
+  </si>
+  <si>
+    <t>Final Project + Reproducibility</t>
+  </si>
+  <si>
+    <t>GONE AT SDSS</t>
+  </si>
+  <si>
+    <t>Diagram NYT Articles</t>
+  </si>
+  <si>
+    <t>Data Descriptions</t>
+  </si>
+  <si>
+    <t>Data Journalism</t>
+  </si>
+  <si>
+    <t>Spreadsheets, Summaries, and Pivot Tables</t>
+  </si>
+  <si>
+    <t>One Number Stories</t>
+  </si>
+  <si>
+    <t>Table Design</t>
+  </si>
+  <si>
+    <t>Peer Review of One-number Stories</t>
+  </si>
+  <si>
+    <t>Peer Review One Number Story</t>
+  </si>
+  <si>
+    <t>How to Read a Research Paper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://sites.google.com/wfu.edu/uscots23/home </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.causeweb.org/cause/sites/default/files/ecots/ecots22/materials/NUZZO-USCOTS-keynote-2023-June2.pdf </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/document/u/0/d/1O6rJUi9BcnfkxJV77flu6r7V9X6G7ePqK1L5t8e0P8w/mobilebasic </t>
+  </si>
+  <si>
+    <t>Form Teams, Select Data from Tidy Tuesday</t>
+  </si>
+  <si>
+    <t>Initial Data Proposals</t>
+  </si>
+  <si>
+    <t>Bad Graphics Day</t>
+  </si>
+  <si>
+    <t>Booster Conditions</t>
+  </si>
+  <si>
+    <t>NYT What's Going on with this Graph</t>
+  </si>
+  <si>
+    <t>Copy the Masters</t>
+  </si>
+  <si>
+    <t>Florence Nightingale</t>
+  </si>
+  <si>
+    <t>Cover letter</t>
+  </si>
+  <si>
+    <t>Make your own website</t>
+  </si>
+  <si>
+    <t>Activities</t>
+  </si>
+  <si>
+    <t>Visit from Career Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://slowrevealgraphs.com/#:~:text=What%20IS%20a%20Slow%20Reveal,beyond)%20make%20sense%20of%20data. </t>
+  </si>
+  <si>
+    <t>Intro/History of Viz</t>
+  </si>
+  <si>
+    <t>Accessibility/Colors/Principles/Perception</t>
+  </si>
+  <si>
+    <t>https://history.infowetrust.com/</t>
+  </si>
+  <si>
+    <t>Jigsaw History of Graphics</t>
+  </si>
+  <si>
+    <t>Begin One Number Story</t>
+  </si>
+  <si>
+    <t>Data Selection + Proposals</t>
+  </si>
+  <si>
+    <t>Storyboarding</t>
+  </si>
+  <si>
+    <t>Storyboarding in Groups</t>
+  </si>
+  <si>
+    <t>Finding Internships + Online Presence/Career Panel</t>
+  </si>
+  <si>
+    <t>Team Storyboard</t>
+  </si>
+  <si>
+    <t>Final Report Draft</t>
+  </si>
+  <si>
+    <t>Final Report Revisions</t>
+  </si>
+  <si>
+    <t>Stand Alone Graphic</t>
+  </si>
+  <si>
+    <t>Data Viz Makovers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.storytellingwithdata.com/blog?category=Makeovers </t>
+  </si>
+  <si>
+    <t>Redesign your graphic</t>
+  </si>
+  <si>
+    <t>Stat 150 Prompts (Soma)</t>
+  </si>
+  <si>
+    <t>Understanding the Publication Process</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -643,6 +776,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -658,7 +799,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -726,11 +867,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -767,8 +920,31 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -782,10 +958,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1050,619 +1222,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06962521-CB75-4304-97E8-060BEAF42701}">
-  <dimension ref="A1:H47"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="10.109375" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="70" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="72.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="21"/>
-      <c r="F2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>45019</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="F6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E7" s="22" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>45021</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="H8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="18"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>45026</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="G10" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>45028</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="18" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>45033</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="F14" t="s">
-        <v>155</v>
-      </c>
-      <c r="H14" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F15" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>45035</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
-        <v>45040</v>
-      </c>
-      <c r="B18">
-        <v>4</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="F18" t="s">
-        <v>173</v>
-      </c>
-      <c r="H18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E19" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="H19" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
-        <v>45042</v>
-      </c>
-      <c r="B20">
-        <v>4</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="F20" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
-        <v>45047</v>
-      </c>
-      <c r="B22">
-        <v>5</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="F22" t="s">
-        <v>168</v>
-      </c>
-      <c r="G22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E23" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="F23" t="s">
-        <v>172</v>
-      </c>
-      <c r="G23" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
-        <v>45049</v>
-      </c>
-      <c r="B24">
-        <v>5</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
-        <v>45054</v>
-      </c>
-      <c r="B26">
-        <v>6</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="H26" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
-        <v>45056</v>
-      </c>
-      <c r="B28">
-        <v>6</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
-        <v>45061</v>
-      </c>
-      <c r="B30">
-        <v>7</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C31" s="9"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="3">
-        <v>45063</v>
-      </c>
-      <c r="B32">
-        <v>7</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="F32" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="18"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="3">
-        <v>45068</v>
-      </c>
-      <c r="B34">
-        <v>8</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G34" t="s">
-        <v>126</v>
-      </c>
-      <c r="H34" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G35" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="3">
-        <v>45070</v>
-      </c>
-      <c r="B36">
-        <v>8</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="18"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="3">
-        <v>45075</v>
-      </c>
-      <c r="B38">
-        <v>9</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="3">
-        <v>45077</v>
-      </c>
-      <c r="B40">
-        <v>9</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="3">
-        <v>45082</v>
-      </c>
-      <c r="B42">
-        <v>10</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="H42" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H43" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="3">
-        <v>45084</v>
-      </c>
-      <c r="B44">
-        <v>10</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="23"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M71"/>
   <sheetViews>
@@ -2635,7 +2194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA95240-CF41-4C58-AE91-D8561390A525}">
   <dimension ref="A1:H7"/>
   <sheetViews>
@@ -2750,4 +2309,1164 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06962521-CB75-4304-97E8-060BEAF42701}">
+  <dimension ref="A1:H47"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="70" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="72.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="21"/>
+      <c r="F2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>45019</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="F6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E7" s="22" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>45021</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="H8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="18"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>45026</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="G10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>45028</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>45033</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="F14" t="s">
+        <v>155</v>
+      </c>
+      <c r="H14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>45035</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>45040</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="F18" t="s">
+        <v>173</v>
+      </c>
+      <c r="H18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E19" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="H19" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>45042</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="F20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>45047</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="F22" t="s">
+        <v>168</v>
+      </c>
+      <c r="G22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E23" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="F23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G23" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>45049</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>45054</v>
+      </c>
+      <c r="B26">
+        <v>6</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="H26" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>45056</v>
+      </c>
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>45061</v>
+      </c>
+      <c r="B30">
+        <v>7</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C31" s="9"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>45063</v>
+      </c>
+      <c r="B32">
+        <v>7</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F32" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="18"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>45068</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" t="s">
+        <v>126</v>
+      </c>
+      <c r="H34" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G35" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>45070</v>
+      </c>
+      <c r="B36">
+        <v>8</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="18"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
+        <v>45075</v>
+      </c>
+      <c r="B38">
+        <v>9</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>45077</v>
+      </c>
+      <c r="B40">
+        <v>9</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="E41" s="23"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
+        <v>45082</v>
+      </c>
+      <c r="B42">
+        <v>10</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="H42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H43" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
+        <v>45084</v>
+      </c>
+      <c r="B44">
+        <v>10</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09C1700-718F-4A1F-822B-8D86B7CD7ADC}">
+  <dimension ref="A1:I45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="70" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="72.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27">
+        <v>45019</v>
+      </c>
+      <c r="B2" s="26">
+        <v>1</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="5"/>
+      <c r="E3" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27">
+        <v>45390</v>
+      </c>
+      <c r="B4" s="26">
+        <v>2</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="26" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="28"/>
+      <c r="E5" s="29"/>
+    </row>
+    <row r="6" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27">
+        <v>45026</v>
+      </c>
+      <c r="B6" s="26">
+        <v>2</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="E6" s="29"/>
+      <c r="F6" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="5"/>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="8" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27">
+        <v>45397</v>
+      </c>
+      <c r="B8" s="26">
+        <v>3</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="28"/>
+      <c r="E9" s="36" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="27">
+        <v>45399</v>
+      </c>
+      <c r="B10" s="26">
+        <v>3</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="E10" s="29"/>
+      <c r="F10" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="G10" s="31"/>
+    </row>
+    <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="5"/>
+      <c r="E11" s="23"/>
+    </row>
+    <row r="12" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27">
+        <v>45404</v>
+      </c>
+      <c r="B12" s="26">
+        <v>4</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="28"/>
+      <c r="E13" s="36"/>
+    </row>
+    <row r="14" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="27">
+        <v>45406</v>
+      </c>
+      <c r="B14" s="26">
+        <v>4</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="5"/>
+      <c r="E15" s="23"/>
+    </row>
+    <row r="16" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="27">
+        <v>45411</v>
+      </c>
+      <c r="B16" s="26">
+        <v>5</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="28"/>
+      <c r="E17" s="29"/>
+      <c r="I17" s="26" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="27">
+        <v>45413</v>
+      </c>
+      <c r="B18" s="26">
+        <v>5</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="E18" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="5"/>
+      <c r="E19" s="23"/>
+    </row>
+    <row r="20" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="27">
+        <v>45418</v>
+      </c>
+      <c r="B20" s="26">
+        <v>6</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="28"/>
+      <c r="E21" s="29"/>
+    </row>
+    <row r="22" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="27">
+        <v>45420</v>
+      </c>
+      <c r="B22" s="26">
+        <v>6</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="E22" s="36" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="5"/>
+      <c r="E23" s="23"/>
+    </row>
+    <row r="24" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="27">
+        <v>45425</v>
+      </c>
+      <c r="B24" s="26">
+        <v>7</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="E24" s="36"/>
+      <c r="F24" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="H24" s="31" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="28"/>
+      <c r="E25" s="29"/>
+    </row>
+    <row r="26" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="27">
+        <v>45427</v>
+      </c>
+      <c r="B26" s="26">
+        <v>7</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="E26" s="29"/>
+    </row>
+    <row r="27" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="32"/>
+      <c r="E27" s="23"/>
+    </row>
+    <row r="28" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="27">
+        <v>45432</v>
+      </c>
+      <c r="B28" s="26">
+        <v>8</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="E28" s="29"/>
+      <c r="G28" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="I28" s="26" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="28"/>
+      <c r="E29" s="29"/>
+      <c r="I29" s="26" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="27">
+        <v>45434</v>
+      </c>
+      <c r="B30" s="26">
+        <v>8</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="E30" s="29"/>
+      <c r="G30" s="26" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="5"/>
+      <c r="E31" s="23"/>
+    </row>
+    <row r="32" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="27">
+        <v>45440</v>
+      </c>
+      <c r="B32" s="26">
+        <v>9</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="E32" s="29"/>
+      <c r="G32" s="30"/>
+    </row>
+    <row r="33" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="28"/>
+      <c r="E33" s="29"/>
+    </row>
+    <row r="34" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="27">
+        <v>45441</v>
+      </c>
+      <c r="B34" s="26">
+        <v>9</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="E34" s="29"/>
+      <c r="H34" s="26" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="5"/>
+      <c r="E35" s="23"/>
+    </row>
+    <row r="36" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="27">
+        <v>45446</v>
+      </c>
+      <c r="B36" s="26">
+        <v>10</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="E36" s="29"/>
+    </row>
+    <row r="37" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="28"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="29"/>
+    </row>
+    <row r="38" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="33">
+        <v>45448</v>
+      </c>
+      <c r="B38" s="4">
+        <v>10</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="E38" s="23"/>
+    </row>
+    <row r="39" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="40"/>
+      <c r="H39" s="38" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="27"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="29"/>
+    </row>
+    <row r="41" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="28"/>
+      <c r="E41" s="29"/>
+    </row>
+    <row r="42" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="28"/>
+      <c r="E42" s="29"/>
+    </row>
+    <row r="43" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="28"/>
+      <c r="E43" s="29"/>
+    </row>
+    <row r="44" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="28"/>
+      <c r="E44" s="29"/>
+    </row>
+    <row r="45" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="28"/>
+      <c r="E45" s="29"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E9" r:id="rId1" xr:uid="{A8EFD892-0A3D-4F3C-A4BF-FB2138E6A85C}"/>
+    <hyperlink ref="E12" r:id="rId2" xr:uid="{45E7F8F2-0FD1-4368-A025-9997172C0582}"/>
+    <hyperlink ref="E18" r:id="rId3" location=":~:text=What%20IS%20a%20Slow%20Reveal,beyond)%20make%20sense%20of%20data. " xr:uid="{9C088292-D46A-4DFA-8EAC-6A164731AE8C}"/>
+    <hyperlink ref="E16" r:id="rId4" xr:uid="{69FC8AF5-8C2D-4E40-924A-57E5B33EE3B0}"/>
+    <hyperlink ref="E22" r:id="rId5" xr:uid="{6C67902F-AF4F-46D3-A15A-4644DB8C4450}"/>
+    <hyperlink ref="E20" r:id="rId6" xr:uid="{768B11DC-2373-42FD-8E82-439E48B05CF3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
+</worksheet>
 </file>
</xml_diff>